<commit_message>
added 5081 week2 data
</commit_message>
<xml_diff>
--- a/data/5MD.xlsx
+++ b/data/5MD.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14780" windowHeight="11540" tabRatio="500"/>
+    <workbookView xWindow="-320" yWindow="0" windowWidth="20820" windowHeight="14460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="14">
   <si>
     <t>class</t>
   </si>
@@ -58,13 +58,16 @@
   </si>
   <si>
     <t>lost</t>
+  </si>
+  <si>
+    <t>the grime reaper</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -82,6 +85,12 @@
       <u/>
       <sz val="12"/>
       <color theme="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -103,7 +112,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="17">
+  <cellStyleXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -121,12 +130,20 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="16" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="17">
+  <cellStyles count="23">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -135,6 +152,9 @@
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -143,6 +163,9 @@
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -472,10 +495,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -743,6 +766,84 @@
         <v>4</v>
       </c>
     </row>
+    <row r="11" spans="1:8">
+      <c r="A11" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11">
+        <v>2</v>
+      </c>
+      <c r="C11" s="1">
+        <v>43719</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11">
+        <v>3</v>
+      </c>
+      <c r="F11" t="s">
+        <v>9</v>
+      </c>
+      <c r="G11">
+        <v>93</v>
+      </c>
+      <c r="H11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12">
+        <v>2</v>
+      </c>
+      <c r="C12" s="1">
+        <v>43719</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E12">
+        <v>4</v>
+      </c>
+      <c r="F12" t="s">
+        <v>9</v>
+      </c>
+      <c r="G12">
+        <v>59</v>
+      </c>
+      <c r="H12">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13" s="1">
+        <v>43719</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" s="3">
+        <v>4</v>
+      </c>
+      <c r="F13" t="s">
+        <v>9</v>
+      </c>
+      <c r="G13">
+        <v>2</v>
+      </c>
+      <c r="H13">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>